<commit_message>
adding change to excel
</commit_message>
<xml_diff>
--- a/layouts/layout.xlsx
+++ b/layouts/layout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Joses_Stuff/github/keyboard_layout_config_mapper/kinesis2/layouts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Joses_Stuff/github/keyboard_layout_config_mapper/layouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A443C66-CF8A-AB44-9699-1A53C6EDDC45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0576CC-8302-4644-8D72-C6D2B1C20F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enegram-en" sheetId="1" r:id="rId1"/>
@@ -1766,8 +1766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9058,8 +9058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding new hands down inspire variation
</commit_message>
<xml_diff>
--- a/layouts/layout.xlsx
+++ b/layouts/layout.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Joses_Stuff/github/keyboard_layout_config_mapper/layouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0576CC-8302-4644-8D72-C6D2B1C20F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3F7B4C-C84D-2F46-80FD-A2023B01DBF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="enegram-en" sheetId="1" r:id="rId1"/>
-    <sheet name="enegram_dvorak" sheetId="9" r:id="rId2"/>
-    <sheet name="enegram_halmak" sheetId="8" r:id="rId3"/>
-    <sheet name="enegram_eng_spanish_edit" sheetId="6" r:id="rId4"/>
-    <sheet name="English Ranking" sheetId="4" r:id="rId5"/>
-    <sheet name="Spanish Ranking Deduded" sheetId="7" r:id="rId6"/>
+    <sheet name="enegram_handsdown_inspired" sheetId="10" r:id="rId2"/>
+    <sheet name="enegram_dvorak" sheetId="9" r:id="rId3"/>
+    <sheet name="enegram_halmak" sheetId="8" r:id="rId4"/>
+    <sheet name="enegram_eng_spanish_edit" sheetId="6" r:id="rId5"/>
+    <sheet name="English Ranking" sheetId="4" r:id="rId6"/>
+    <sheet name="Spanish Ranking Deduded" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="90">
   <si>
     <t>E 445</t>
   </si>
@@ -304,6 +305,12 @@
   <si>
     <t>Orig 333</t>
   </si>
+  <si>
+    <t>Edit What if inspired #6</t>
+  </si>
+  <si>
+    <t>Orig 396</t>
+  </si>
 </sst>
 </file>
 
@@ -465,7 +472,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -705,6 +712,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -881,7 +894,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -917,6 +930,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -976,6 +991,99 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA5D9AA-94C6-E340-BA80-08333B7F79E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12433300" y="11049000"/>
+          <a:ext cx="13030200" cy="5727700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>3062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{143B115C-D09E-214C-8B93-8C4D558491C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12522200" y="5552962"/>
+          <a:ext cx="11950700" cy="5140438"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1763,6 +1871,1444 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEF181E-BD5E-394B-B30E-64531238E4B6}">
+  <dimension ref="A1:S55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1">
+        <v>272</v>
+      </c>
+      <c r="D1" s="1">
+        <v>97</v>
+      </c>
+      <c r="G1" s="1">
+        <v>145</v>
+      </c>
+      <c r="H1" s="1">
+        <v>136</v>
+      </c>
+      <c r="I1" s="1">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1">
+        <v>38</v>
+      </c>
+      <c r="K1">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>119</v>
+      </c>
+      <c r="B2" s="1">
+        <v>270</v>
+      </c>
+      <c r="C2" s="1">
+        <v>445</v>
+      </c>
+      <c r="D2" s="1">
+        <v>287</v>
+      </c>
+      <c r="G2" s="1">
+        <v>180</v>
+      </c>
+      <c r="H2" s="1">
+        <v>331</v>
+      </c>
+      <c r="I2" s="1">
+        <v>232</v>
+      </c>
+      <c r="J2" s="1">
+        <v>258</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="O2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2">
+        <f>_xlfn.XLOOKUP(P2,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>67</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1">
+        <v>224</v>
+      </c>
+      <c r="H3" s="1">
+        <v>90</v>
+      </c>
+      <c r="I3" s="1">
+        <v>86</v>
+      </c>
+      <c r="J3" s="1">
+        <v>76</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3">
+        <f>_xlfn.XLOOKUP(P3,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>SUM(A1:A3)</f>
+        <v>239</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:D4" si="0">SUM(B1:B3)</f>
+        <v>337</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>723</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>403</v>
+      </c>
+      <c r="E4">
+        <f>SUM(A4:D4)</f>
+        <v>1702</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:K4" si="1">SUM(G1:G3)</f>
+        <v>549</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>557</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>378</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>372</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <f>SUM(G4:K4)</f>
+        <v>1863</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4">
+        <f>_xlfn.XLOOKUP(P4,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5">
+        <f>_xlfn.XLOOKUP(P5,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6">
+        <f>_xlfn.XLOOKUP(P6,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(A1,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>B</v>
+      </c>
+      <c r="B7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(B1,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>Y</v>
+      </c>
+      <c r="C7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(C1,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>O</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(D1,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>U</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(G1,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>L</v>
+      </c>
+      <c r="H7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(H1,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>D</v>
+      </c>
+      <c r="I7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(I1,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>W</v>
+      </c>
+      <c r="J7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(J1,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>V</v>
+      </c>
+      <c r="K7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(K1,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>Z</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7">
+        <f>_xlfn.XLOOKUP(P7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(A2,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>C</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(B2,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>I</v>
+      </c>
+      <c r="C8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(C2,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>E</v>
+      </c>
+      <c r="D8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(D2,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>A</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(G2,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>H</v>
+      </c>
+      <c r="H8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(H2,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>T</v>
+      </c>
+      <c r="I8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(I2,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>S</v>
+      </c>
+      <c r="J8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(J2,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>N</v>
+      </c>
+      <c r="K8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(K2,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>Q</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8">
+        <f>_xlfn.XLOOKUP(P8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(A3,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>G</v>
+      </c>
+      <c r="B9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(B3,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>X</v>
+      </c>
+      <c r="C9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(C3,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>J</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(D3,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>K</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(G3,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>R</v>
+      </c>
+      <c r="H9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(H3,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>M</v>
+      </c>
+      <c r="I9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(I3,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>F</v>
+      </c>
+      <c r="J9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(J3,'English Ranking'!$C$1:$C$26,'English Ranking'!$B$1:$B$26)</f>
+        <v>P</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="O9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R9">
+        <f>_xlfn.XLOOKUP(P9,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10">
+        <f>_xlfn.XLOOKUP(P10,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="R11">
+        <f>_xlfn.XLOOKUP(P11,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="R12">
+        <f>_xlfn.XLOOKUP(P12,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <f>_xlfn.XLOOKUP(A7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>55</v>
+      </c>
+      <c r="B13" s="4">
+        <f>_xlfn.XLOOKUP(B7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>55</v>
+      </c>
+      <c r="C13" s="4">
+        <f>_xlfn.XLOOKUP(C7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+      <c r="D13" s="4">
+        <f>_xlfn.XLOOKUP(D7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>89</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E15" si="2">SUM(A13:D13)</f>
+        <v>432</v>
+      </c>
+      <c r="G13" s="4">
+        <f>_xlfn.XLOOKUP(G7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>144</v>
+      </c>
+      <c r="H13" s="4">
+        <f>_xlfn.XLOOKUP(H7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>144</v>
+      </c>
+      <c r="I13" s="4">
+        <f>_xlfn.XLOOKUP(I7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>55</v>
+      </c>
+      <c r="J13" s="4">
+        <f>_xlfn.XLOOKUP(J7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>34</v>
+      </c>
+      <c r="K13" s="4">
+        <f>_xlfn.XLOOKUP(K7,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L13:L15" si="3">SUM(G13:K13)</f>
+        <v>380</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="R13">
+        <f>_xlfn.XLOOKUP(P13,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <f>_xlfn.XLOOKUP(A8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>144</v>
+      </c>
+      <c r="B14" s="4">
+        <f>_xlfn.XLOOKUP(B8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+      <c r="C14" s="4">
+        <f>_xlfn.XLOOKUP(C8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>377</v>
+      </c>
+      <c r="D14" s="4">
+        <f>_xlfn.XLOOKUP(D8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>987</v>
+      </c>
+      <c r="G14" s="4">
+        <f>_xlfn.XLOOKUP(G8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>144</v>
+      </c>
+      <c r="H14" s="4">
+        <f>_xlfn.XLOOKUP(H8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>377</v>
+      </c>
+      <c r="I14" s="4">
+        <f>_xlfn.XLOOKUP(I8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+      <c r="J14" s="4">
+        <f>_xlfn.XLOOKUP(J8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+      <c r="K14" s="4">
+        <f>_xlfn.XLOOKUP(K8,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>3</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>990</v>
+      </c>
+      <c r="O14" s="11"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <f>_xlfn.XLOOKUP(A9,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>55</v>
+      </c>
+      <c r="B15" s="4">
+        <f>_xlfn.XLOOKUP(B9,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>8</v>
+      </c>
+      <c r="C15" s="4">
+        <f>_xlfn.XLOOKUP(C9,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>5</v>
+      </c>
+      <c r="D15" s="4">
+        <f>_xlfn.XLOOKUP(D9,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>21</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+      <c r="G15" s="4">
+        <f>_xlfn.XLOOKUP(G9,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+      <c r="H15" s="4">
+        <f>_xlfn.XLOOKUP(H9,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>89</v>
+      </c>
+      <c r="I15" s="4">
+        <f>_xlfn.XLOOKUP(I9,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>89</v>
+      </c>
+      <c r="J15" s="4">
+        <f>_xlfn.XLOOKUP(J9,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>89</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15">
+        <f>_xlfn.XLOOKUP(P15,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f>SUM(A13:A15)</f>
+        <v>254</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:D16" si="4">SUM(B13:B15)</f>
+        <v>296</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="4"/>
+        <v>615</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="4"/>
+        <v>343</v>
+      </c>
+      <c r="E16">
+        <f>SUM(A16:D16)</f>
+        <v>1508</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:K16" si="5">SUM(G13:G15)</f>
+        <v>521</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="5"/>
+        <v>610</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>377</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>356</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <f>SUM(G16:K16)</f>
+        <v>1870</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R16">
+        <f>_xlfn.XLOOKUP(P16,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="R17">
+        <f>_xlfn.XLOOKUP(P17,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="R18">
+        <f>_xlfn.XLOOKUP(P18,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P19" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="R19">
+        <f>_xlfn.XLOOKUP(P19,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="R20">
+        <f>_xlfn.XLOOKUP(P20,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O21" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="R21">
+        <f>_xlfn.XLOOKUP(P21,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="P22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q22" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="R22">
+        <f>_xlfn.XLOOKUP(P22,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="R23">
+        <f>_xlfn.XLOOKUP(P23,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O24" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q24" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R24">
+        <f>_xlfn.XLOOKUP(P24,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O25" t="s">
+        <v>31</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R25">
+        <f>_xlfn.XLOOKUP(P25,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O26" t="s">
+        <v>41</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R26">
+        <f>_xlfn.XLOOKUP(P26,'English Ranking'!$B$1:$B$26,'English Ranking'!$D$1:$D$26)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O28" t="s">
+        <v>51</v>
+      </c>
+      <c r="P28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O29" t="s">
+        <v>50</v>
+      </c>
+      <c r="P29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" t="s">
+        <v>75</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <f>_xlfn.XLOOKUP(A33,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="B40" s="4">
+        <f>_xlfn.XLOOKUP(B33,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="C40" s="4">
+        <f>_xlfn.XLOOKUP(C33,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="4">
+        <f>_xlfn.XLOOKUP(D33,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ref="E40:E44" si="6">SUM(A40:D40)</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="4">
+        <f>_xlfn.XLOOKUP(G33,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="4">
+        <f>_xlfn.XLOOKUP(D37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>3</v>
+      </c>
+      <c r="I40" s="4">
+        <f>_xlfn.XLOOKUP(I33,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="4">
+        <f>_xlfn.XLOOKUP(J33,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <f t="shared" ref="L40:L43" si="7">SUM(G40:K40)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <f>_xlfn.XLOOKUP(A34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>55</v>
+      </c>
+      <c r="B41" s="4">
+        <f>_xlfn.XLOOKUP(B34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>89</v>
+      </c>
+      <c r="C41" s="4">
+        <f>_xlfn.XLOOKUP(C34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>89</v>
+      </c>
+      <c r="D41" s="4">
+        <f>_xlfn.XLOOKUP(D34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>144</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="6"/>
+        <v>377</v>
+      </c>
+      <c r="G41" s="4">
+        <f>_xlfn.XLOOKUP(G34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>89</v>
+      </c>
+      <c r="H41" s="4">
+        <f>_xlfn.XLOOKUP(H34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="I41" s="4">
+        <f>_xlfn.XLOOKUP(I34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>55</v>
+      </c>
+      <c r="J41" s="4">
+        <f>_xlfn.XLOOKUP(J34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>89</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="7"/>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <f>_xlfn.XLOOKUP(A35,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="B42" s="4">
+        <f>_xlfn.XLOOKUP(B35,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="C42" s="4">
+        <f>_xlfn.XLOOKUP(C35,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>377</v>
+      </c>
+      <c r="D42" s="4">
+        <f>_xlfn.XLOOKUP(D35,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="6"/>
+        <v>1076</v>
+      </c>
+      <c r="G42" s="4">
+        <f>_xlfn.XLOOKUP(G35,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="H42" s="4">
+        <f>_xlfn.XLOOKUP(H35,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>377</v>
+      </c>
+      <c r="I42" s="4">
+        <f>_xlfn.XLOOKUP(I35,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="J42" s="4">
+        <f>_xlfn.XLOOKUP(J35,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>144</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="7"/>
+        <v>987</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <f>_xlfn.XLOOKUP(A36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>34</v>
+      </c>
+      <c r="B43" s="4">
+        <f>_xlfn.XLOOKUP(B36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>55</v>
+      </c>
+      <c r="C43" s="4">
+        <f>_xlfn.XLOOKUP(C36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>144</v>
+      </c>
+      <c r="D43" s="4">
+        <f>_xlfn.XLOOKUP(D36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>144</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="6"/>
+        <v>377</v>
+      </c>
+      <c r="G43" s="4">
+        <f>_xlfn.XLOOKUP(G36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>21</v>
+      </c>
+      <c r="H43" s="4">
+        <f>_xlfn.XLOOKUP(H36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>5</v>
+      </c>
+      <c r="I43" s="4">
+        <f>_xlfn.XLOOKUP(I36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>8</v>
+      </c>
+      <c r="J43" s="4">
+        <f>_xlfn.XLOOKUP(J36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>55</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <f>_xlfn.XLOOKUP(A37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="B44" s="4">
+        <f>_xlfn.XLOOKUP(B37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
+        <f>_xlfn.XLOOKUP(C37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>3</v>
+      </c>
+      <c r="D44" s="4">
+        <f>_xlfn.XLOOKUP(D37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ref="G44:J44" si="8">SUM(G41:G43)</f>
+        <v>343</v>
+      </c>
+      <c r="H44">
+        <f>SUM(H40:H43)</f>
+        <v>618</v>
+      </c>
+      <c r="I44">
+        <f>SUM(I40:I43)</f>
+        <v>296</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="8"/>
+        <v>288</v>
+      </c>
+      <c r="L44">
+        <f>SUM(L40:L43)</f>
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f>SUM(A41:A44)</f>
+        <v>322</v>
+      </c>
+      <c r="B45">
+        <f>SUM(B40:B44)</f>
+        <v>377</v>
+      </c>
+      <c r="C45">
+        <f>SUM(C40:C44)</f>
+        <v>613</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ref="D45:E45" si="9">SUM(D41:D44)</f>
+        <v>524</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="9"/>
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <f>_xlfn.XLOOKUP(A33,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="B48" s="4">
+        <f>_xlfn.XLOOKUP(B33,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="4">
+        <f>_xlfn.XLOOKUP(C33,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="4">
+        <f>_xlfn.XLOOKUP(D33,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ref="E48:E52" si="10">SUM(A48:D48)</f>
+        <v>0</v>
+      </c>
+      <c r="G48" s="4">
+        <f>_xlfn.XLOOKUP(G33,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="4">
+        <f>_xlfn.XLOOKUP(H33,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="I48" s="4">
+        <f>_xlfn.XLOOKUP(I33,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="J48" s="4">
+        <f>_xlfn.XLOOKUP(J33,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <f t="shared" ref="L48:L51" si="11">SUM(G48:K48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <f>_xlfn.XLOOKUP(A34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>53</v>
+      </c>
+      <c r="B49" s="4">
+        <f>_xlfn.XLOOKUP(B34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>86</v>
+      </c>
+      <c r="C49" s="4">
+        <f>_xlfn.XLOOKUP(C34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>90</v>
+      </c>
+      <c r="D49" s="4">
+        <f>_xlfn.XLOOKUP(D34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>119</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="10"/>
+        <v>348</v>
+      </c>
+      <c r="G49" s="4">
+        <f>_xlfn.XLOOKUP(G34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>97</v>
+      </c>
+      <c r="H49" s="4">
+        <f>_xlfn.XLOOKUP(H34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>272</v>
+      </c>
+      <c r="I49" s="4">
+        <f>_xlfn.XLOOKUP(I34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>59</v>
+      </c>
+      <c r="J49" s="4">
+        <f>_xlfn.XLOOKUP(J34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>76</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="11"/>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <f>_xlfn.XLOOKUP(A35,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>258</v>
+      </c>
+      <c r="B50" s="4">
+        <f>_xlfn.XLOOKUP(B35,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>232</v>
+      </c>
+      <c r="C50" s="4">
+        <f>_xlfn.XLOOKUP(C35,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>331</v>
+      </c>
+      <c r="D50" s="4">
+        <f>_xlfn.XLOOKUP(D35,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>224</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="10"/>
+        <v>1045</v>
+      </c>
+      <c r="G50" s="4">
+        <f>_xlfn.XLOOKUP(G35,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>287</v>
+      </c>
+      <c r="H50" s="4">
+        <f>_xlfn.XLOOKUP(H35,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>445</v>
+      </c>
+      <c r="I50" s="4">
+        <f>_xlfn.XLOOKUP(I35,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>270</v>
+      </c>
+      <c r="J50" s="4">
+        <f>_xlfn.XLOOKUP(J35,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>180</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="11"/>
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <f>_xlfn.XLOOKUP(A36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>38</v>
+      </c>
+      <c r="B51" s="4">
+        <f>_xlfn.XLOOKUP(B36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>60</v>
+      </c>
+      <c r="C51" s="4">
+        <f>_xlfn.XLOOKUP(C36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>136</v>
+      </c>
+      <c r="D51" s="4">
+        <f>_xlfn.XLOOKUP(D36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>145</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="10"/>
+        <v>379</v>
+      </c>
+      <c r="G51" s="4">
+        <f>_xlfn.XLOOKUP(G36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>19</v>
+      </c>
+      <c r="H51" s="4">
+        <f>_xlfn.XLOOKUP(H36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>6</v>
+      </c>
+      <c r="I51" s="4">
+        <f>_xlfn.XLOOKUP(I36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>8</v>
+      </c>
+      <c r="J51" s="4">
+        <f>_xlfn.XLOOKUP(J36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>67</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="11"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <f>_xlfn.XLOOKUP(A37,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="B52" s="4">
+        <f>_xlfn.XLOOKUP(B37,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="4">
+        <f>_xlfn.XLOOKUP(C37,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>3</v>
+      </c>
+      <c r="D52" s="4">
+        <f>_xlfn.XLOOKUP(D37,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>4</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="G52">
+        <f t="shared" ref="G52" si="12">SUM(G49:G51)</f>
+        <v>403</v>
+      </c>
+      <c r="H52">
+        <f>SUM(H48:H51)</f>
+        <v>723</v>
+      </c>
+      <c r="I52">
+        <f>SUM(I48:I51)</f>
+        <v>337</v>
+      </c>
+      <c r="J52">
+        <f t="shared" ref="J52" si="13">SUM(J49:J51)</f>
+        <v>323</v>
+      </c>
+      <c r="L52">
+        <f>SUM(G52:K52)</f>
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f>SUM(A49:A52)</f>
+        <v>349</v>
+      </c>
+      <c r="B53">
+        <f>SUM(B48:B52)</f>
+        <v>378</v>
+      </c>
+      <c r="C53">
+        <f>SUM(C48:C52)</f>
+        <v>560</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ref="D53:E53" si="14">SUM(D49:D52)</f>
+        <v>492</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="14"/>
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="I54" t="s">
+        <v>89</v>
+      </c>
+      <c r="J54" t="s">
+        <v>87</v>
+      </c>
+      <c r="S54" s="22"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55">
+        <v>1856</v>
+      </c>
+      <c r="K55" t="s">
+        <v>81</v>
+      </c>
+      <c r="L55">
+        <v>1706</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S122"/>
   <sheetViews>
@@ -5006,7 +6552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R87"/>
   <sheetViews>
@@ -7198,7 +8744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L53"/>
   <sheetViews>
@@ -8271,7 +9817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O27"/>
   <sheetViews>
@@ -9054,11 +10600,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding new config that match what i am using
</commit_message>
<xml_diff>
--- a/layouts/layout.xlsx
+++ b/layouts/layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Joses_Stuff/github/keyboard_layout_config_mapper/layouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3F7B4C-C84D-2F46-80FD-A2023B01DBF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40B119F-7204-ED4E-8A53-7A087091FB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="91">
   <si>
     <t>E 445</t>
   </si>
@@ -311,6 +311,9 @@
   <si>
     <t>Orig 396</t>
   </si>
+  <si>
+    <t>Edit What if inspired #7</t>
+  </si>
 </sst>
 </file>
 
@@ -472,7 +475,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -718,6 +721,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -894,7 +903,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -932,6 +941,7 @@
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1039,15 +1049,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>3062</xdr:rowOff>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>79262</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1070,7 +1080,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12522200" y="5552962"/>
+          <a:off x="12509500" y="6035562"/>
           <a:ext cx="11950700" cy="5140438"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1872,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEF181E-BD5E-394B-B30E-64531238E4B6}">
-  <dimension ref="A1:S55"/>
+  <dimension ref="A1:S82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2682,7 +2692,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -2710,16 +2720,16 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="27" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -2733,7 +2743,7 @@
         <v>44</v>
       </c>
       <c r="J34" s="28" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -2746,7 +2756,7 @@
       <c r="C35" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="29" t="s">
         <v>33</v>
       </c>
       <c r="E35" s="11"/>
@@ -2760,22 +2770,22 @@
       <c r="I35" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="27" t="s">
-        <v>34</v>
+      <c r="J35" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>34</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -2794,14 +2804,16 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="C37" s="25" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -2836,7 +2848,7 @@
       </c>
       <c r="H40" s="4">
         <f>_xlfn.XLOOKUP(D37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="I40" s="4">
         <f>_xlfn.XLOOKUP(I33,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
@@ -2848,21 +2860,21 @@
       </c>
       <c r="L40">
         <f t="shared" ref="L40:L43" si="7">SUM(G40:K40)</f>
-        <v>3</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <f>_xlfn.XLOOKUP(A34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="B41" s="4">
         <f>_xlfn.XLOOKUP(B34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="C41" s="4">
         <f>_xlfn.XLOOKUP(C34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>89</v>
+        <v>144</v>
       </c>
       <c r="D41" s="4">
         <f>_xlfn.XLOOKUP(D34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
@@ -2870,7 +2882,7 @@
       </c>
       <c r="E41">
         <f t="shared" si="6"/>
-        <v>377</v>
+        <v>343</v>
       </c>
       <c r="G41" s="4">
         <f>_xlfn.XLOOKUP(G34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
@@ -2886,11 +2898,11 @@
       </c>
       <c r="J41" s="4">
         <f>_xlfn.XLOOKUP(J34,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="L41">
         <f t="shared" si="7"/>
-        <v>466</v>
+        <v>377</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -2938,15 +2950,15 @@
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <f>_xlfn.XLOOKUP(A36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="B43" s="4">
         <f>_xlfn.XLOOKUP(B36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="C43" s="4">
         <f>_xlfn.XLOOKUP(C36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="D43" s="4">
         <f>_xlfn.XLOOKUP(D36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
@@ -2954,7 +2966,7 @@
       </c>
       <c r="E43">
         <f t="shared" si="6"/>
-        <v>377</v>
+        <v>411</v>
       </c>
       <c r="G43" s="4">
         <f>_xlfn.XLOOKUP(G36,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
@@ -2980,23 +2992,23 @@
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <f>_xlfn.XLOOKUP(A37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B44" s="4">
         <f>_xlfn.XLOOKUP(B37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C44" s="4">
         <f>_xlfn.XLOOKUP(C37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D44" s="4">
         <f>_xlfn.XLOOKUP(D37,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="E44">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="G44">
         <f t="shared" ref="G44:J44" si="8">SUM(G41:G43)</f>
@@ -3004,7 +3016,7 @@
       </c>
       <c r="H44">
         <f>SUM(H40:H43)</f>
-        <v>618</v>
+        <v>670</v>
       </c>
       <c r="I44">
         <f>SUM(I40:I43)</f>
@@ -3012,33 +3024,33 @@
       </c>
       <c r="J44">
         <f t="shared" si="8"/>
-        <v>288</v>
+        <v>199</v>
       </c>
       <c r="L44">
         <f>SUM(L40:L43)</f>
-        <v>1545</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <f>SUM(A41:A44)</f>
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B45">
         <f>SUM(B40:B44)</f>
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C45">
         <f>SUM(C40:C44)</f>
-        <v>613</v>
+        <v>644</v>
       </c>
       <c r="D45">
         <f t="shared" ref="D45:E45" si="9">SUM(D41:D44)</f>
-        <v>524</v>
+        <v>576</v>
       </c>
       <c r="E45">
         <f t="shared" si="9"/>
-        <v>1836</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -3091,23 +3103,23 @@
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <f>_xlfn.XLOOKUP(A34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B49" s="4">
         <f>_xlfn.XLOOKUP(B34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C49" s="4">
         <f>_xlfn.XLOOKUP(C34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>90</v>
+        <v>136</v>
       </c>
       <c r="D49" s="4">
         <f>_xlfn.XLOOKUP(D34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="E49">
         <f t="shared" si="10"/>
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="G49" s="4">
         <f>_xlfn.XLOOKUP(G34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
@@ -3123,11 +3135,11 @@
       </c>
       <c r="J49" s="4">
         <f>_xlfn.XLOOKUP(J34,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="L49">
         <f t="shared" si="11"/>
-        <v>504</v>
+        <v>428</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
@@ -3165,33 +3177,33 @@
       </c>
       <c r="J50" s="4">
         <f>_xlfn.XLOOKUP(J35,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>180</v>
+        <v>119</v>
       </c>
       <c r="L50">
         <f t="shared" si="11"/>
-        <v>1182</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <f>_xlfn.XLOOKUP(A36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B51" s="4">
         <f>_xlfn.XLOOKUP(B36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C51" s="4">
         <f>_xlfn.XLOOKUP(C36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="D51" s="4">
         <f>_xlfn.XLOOKUP(D36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="E51">
         <f t="shared" si="10"/>
-        <v>379</v>
+        <v>432</v>
       </c>
       <c r="G51" s="4">
         <f>_xlfn.XLOOKUP(G36,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
@@ -3217,23 +3229,23 @@
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <f>_xlfn.XLOOKUP(A37,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B52" s="4">
         <f>_xlfn.XLOOKUP(B37,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C52" s="4">
         <f>_xlfn.XLOOKUP(C37,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="D52" s="4">
         <f>_xlfn.XLOOKUP(D37,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="E52">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G52">
         <f t="shared" ref="G52" si="12">SUM(G49:G51)</f>
@@ -3249,33 +3261,33 @@
       </c>
       <c r="J52">
         <f t="shared" ref="J52" si="13">SUM(J49:J51)</f>
-        <v>323</v>
+        <v>186</v>
       </c>
       <c r="L52">
         <f>SUM(G52:K52)</f>
-        <v>1786</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53">
         <f>SUM(A49:A52)</f>
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="B53">
         <f>SUM(B48:B52)</f>
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C53">
         <f>SUM(C48:C52)</f>
-        <v>560</v>
+        <v>595</v>
       </c>
       <c r="D53">
         <f t="shared" ref="D53:E53" si="14">SUM(D49:D52)</f>
-        <v>492</v>
+        <v>602</v>
       </c>
       <c r="E53">
         <f t="shared" si="14"/>
-        <v>1779</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
@@ -3298,6 +3310,626 @@
         <v>81</v>
       </c>
       <c r="L55">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" t="s">
+        <v>75</v>
+      </c>
+      <c r="G60" t="s">
+        <v>75</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J60" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I61" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J61" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I62" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J62" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A63" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="I63" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J63" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="11"/>
+      <c r="C64" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" s="4">
+        <f>_xlfn.XLOOKUP(A60,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="B67" s="4">
+        <f>_xlfn.XLOOKUP(B60,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="C67" s="4">
+        <f>_xlfn.XLOOKUP(C60,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="D67" s="4">
+        <f>_xlfn.XLOOKUP(D60,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E71" si="15">SUM(A67:D67)</f>
+        <v>0</v>
+      </c>
+      <c r="G67" s="4">
+        <f>_xlfn.XLOOKUP(G60,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="4">
+        <f>_xlfn.XLOOKUP(D64,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>3</v>
+      </c>
+      <c r="I67" s="4">
+        <f>_xlfn.XLOOKUP(I60,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="J67" s="4">
+        <f>_xlfn.XLOOKUP(J60,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <f t="shared" ref="L67:L70" si="16">SUM(G67:K67)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
+        <f>_xlfn.XLOOKUP(A61,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>55</v>
+      </c>
+      <c r="B68" s="4">
+        <f>_xlfn.XLOOKUP(B61,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>89</v>
+      </c>
+      <c r="C68" s="4">
+        <f>_xlfn.XLOOKUP(C61,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>89</v>
+      </c>
+      <c r="D68" s="4">
+        <f>_xlfn.XLOOKUP(D61,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>144</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="15"/>
+        <v>377</v>
+      </c>
+      <c r="G68" s="4">
+        <f>_xlfn.XLOOKUP(G61,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>89</v>
+      </c>
+      <c r="H68" s="4">
+        <f>_xlfn.XLOOKUP(H61,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="I68" s="4">
+        <f>_xlfn.XLOOKUP(I61,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>55</v>
+      </c>
+      <c r="J68" s="4">
+        <f>_xlfn.XLOOKUP(J61,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>89</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="16"/>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69" s="4">
+        <f>_xlfn.XLOOKUP(A62,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="B69" s="4">
+        <f>_xlfn.XLOOKUP(B62,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="C69" s="4">
+        <f>_xlfn.XLOOKUP(C62,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>377</v>
+      </c>
+      <c r="D69" s="4">
+        <f>_xlfn.XLOOKUP(D62,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="15"/>
+        <v>1076</v>
+      </c>
+      <c r="G69" s="4">
+        <f>_xlfn.XLOOKUP(G62,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="H69" s="4">
+        <f>_xlfn.XLOOKUP(H62,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>377</v>
+      </c>
+      <c r="I69" s="4">
+        <f>_xlfn.XLOOKUP(I62,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>233</v>
+      </c>
+      <c r="J69" s="4">
+        <f>_xlfn.XLOOKUP(J62,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>144</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="16"/>
+        <v>987</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="4">
+        <f>_xlfn.XLOOKUP(A63,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>34</v>
+      </c>
+      <c r="B70" s="4">
+        <f>_xlfn.XLOOKUP(B63,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>55</v>
+      </c>
+      <c r="C70" s="4">
+        <f>_xlfn.XLOOKUP(C63,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>144</v>
+      </c>
+      <c r="D70" s="4">
+        <f>_xlfn.XLOOKUP(D63,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>144</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="15"/>
+        <v>377</v>
+      </c>
+      <c r="G70" s="4">
+        <f>_xlfn.XLOOKUP(G63,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>21</v>
+      </c>
+      <c r="H70" s="4">
+        <f>_xlfn.XLOOKUP(H63,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>5</v>
+      </c>
+      <c r="I70" s="4">
+        <f>_xlfn.XLOOKUP(I63,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>8</v>
+      </c>
+      <c r="J70" s="4">
+        <f>_xlfn.XLOOKUP(J63,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>55</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="16"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
+        <f>_xlfn.XLOOKUP(A64,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="B71" s="4">
+        <f>_xlfn.XLOOKUP(B64,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>0</v>
+      </c>
+      <c r="C71" s="4">
+        <f>_xlfn.XLOOKUP(C64,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>3</v>
+      </c>
+      <c r="D71" s="4">
+        <f>_xlfn.XLOOKUP(D64,'English Ranking'!$B$1:$B$30,'English Ranking'!$D$1:$D$30)</f>
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="G71">
+        <f t="shared" ref="G71:J71" si="17">SUM(G68:G70)</f>
+        <v>343</v>
+      </c>
+      <c r="H71">
+        <f>SUM(H67:H70)</f>
+        <v>618</v>
+      </c>
+      <c r="I71">
+        <f>SUM(I67:I70)</f>
+        <v>296</v>
+      </c>
+      <c r="J71">
+        <f t="shared" ref="J71:L71" si="18">SUM(J68:J70)</f>
+        <v>288</v>
+      </c>
+      <c r="L71">
+        <f>SUM(L67:L70)</f>
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <f>SUM(A68:A71)</f>
+        <v>322</v>
+      </c>
+      <c r="B72">
+        <f>SUM(B67:B71)</f>
+        <v>377</v>
+      </c>
+      <c r="C72">
+        <f>SUM(C67:C71)</f>
+        <v>613</v>
+      </c>
+      <c r="D72">
+        <f t="shared" ref="D72:E72" si="19">SUM(D68:D71)</f>
+        <v>524</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="19"/>
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75" s="4">
+        <f>_xlfn.XLOOKUP(A60,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="B75" s="4">
+        <f>_xlfn.XLOOKUP(B60,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="C75" s="4">
+        <f>_xlfn.XLOOKUP(C60,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="D75" s="4">
+        <f>_xlfn.XLOOKUP(D60,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <f t="shared" ref="E75:E79" si="20">SUM(A75:D75)</f>
+        <v>0</v>
+      </c>
+      <c r="G75" s="4">
+        <f>_xlfn.XLOOKUP(G60,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="H75" s="4">
+        <f>_xlfn.XLOOKUP(H60,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="I75" s="4">
+        <f>_xlfn.XLOOKUP(I60,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="J75" s="4">
+        <f>_xlfn.XLOOKUP(J60,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <f t="shared" ref="L75:L78" si="21">SUM(G75:K75)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A76" s="4">
+        <f>_xlfn.XLOOKUP(A61,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>53</v>
+      </c>
+      <c r="B76" s="4">
+        <f>_xlfn.XLOOKUP(B61,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>86</v>
+      </c>
+      <c r="C76" s="4">
+        <f>_xlfn.XLOOKUP(C61,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>90</v>
+      </c>
+      <c r="D76" s="4">
+        <f>_xlfn.XLOOKUP(D61,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>119</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="20"/>
+        <v>348</v>
+      </c>
+      <c r="G76" s="4">
+        <f>_xlfn.XLOOKUP(G61,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>97</v>
+      </c>
+      <c r="H76" s="4">
+        <f>_xlfn.XLOOKUP(H61,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>272</v>
+      </c>
+      <c r="I76" s="4">
+        <f>_xlfn.XLOOKUP(I61,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>59</v>
+      </c>
+      <c r="J76" s="4">
+        <f>_xlfn.XLOOKUP(J61,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>76</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="21"/>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A77" s="4">
+        <f>_xlfn.XLOOKUP(A62,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>258</v>
+      </c>
+      <c r="B77" s="4">
+        <f>_xlfn.XLOOKUP(B62,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>232</v>
+      </c>
+      <c r="C77" s="4">
+        <f>_xlfn.XLOOKUP(C62,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>331</v>
+      </c>
+      <c r="D77" s="4">
+        <f>_xlfn.XLOOKUP(D62,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>224</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="20"/>
+        <v>1045</v>
+      </c>
+      <c r="G77" s="4">
+        <f>_xlfn.XLOOKUP(G62,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>287</v>
+      </c>
+      <c r="H77" s="4">
+        <f>_xlfn.XLOOKUP(H62,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>445</v>
+      </c>
+      <c r="I77" s="4">
+        <f>_xlfn.XLOOKUP(I62,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>270</v>
+      </c>
+      <c r="J77" s="4">
+        <f>_xlfn.XLOOKUP(J62,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>180</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="21"/>
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78" s="4">
+        <f>_xlfn.XLOOKUP(A63,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>38</v>
+      </c>
+      <c r="B78" s="4">
+        <f>_xlfn.XLOOKUP(B63,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>60</v>
+      </c>
+      <c r="C78" s="4">
+        <f>_xlfn.XLOOKUP(C63,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>136</v>
+      </c>
+      <c r="D78" s="4">
+        <f>_xlfn.XLOOKUP(D63,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>145</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="20"/>
+        <v>379</v>
+      </c>
+      <c r="G78" s="4">
+        <f>_xlfn.XLOOKUP(G63,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>19</v>
+      </c>
+      <c r="H78" s="4">
+        <f>_xlfn.XLOOKUP(H63,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>6</v>
+      </c>
+      <c r="I78" s="4">
+        <f>_xlfn.XLOOKUP(I63,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>8</v>
+      </c>
+      <c r="J78" s="4">
+        <f>_xlfn.XLOOKUP(J63,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>67</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="21"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79" s="4">
+        <f>_xlfn.XLOOKUP(A64,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="B79" s="4">
+        <f>_xlfn.XLOOKUP(B64,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>0</v>
+      </c>
+      <c r="C79" s="4">
+        <f>_xlfn.XLOOKUP(C64,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>3</v>
+      </c>
+      <c r="D79" s="4">
+        <f>_xlfn.XLOOKUP(D64,'English Ranking'!$B$1:$B$30,'English Ranking'!$C$1:$C$30)</f>
+        <v>4</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="20"/>
+        <v>7</v>
+      </c>
+      <c r="G79">
+        <f t="shared" ref="G79" si="22">SUM(G76:G78)</f>
+        <v>403</v>
+      </c>
+      <c r="H79">
+        <f>SUM(H75:H78)</f>
+        <v>723</v>
+      </c>
+      <c r="I79">
+        <f>SUM(I75:I78)</f>
+        <v>337</v>
+      </c>
+      <c r="J79">
+        <f t="shared" ref="J79" si="23">SUM(J76:J78)</f>
+        <v>323</v>
+      </c>
+      <c r="L79">
+        <f>SUM(G79:K79)</f>
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <f>SUM(A76:A79)</f>
+        <v>349</v>
+      </c>
+      <c r="B80">
+        <f>SUM(B75:B79)</f>
+        <v>378</v>
+      </c>
+      <c r="C80">
+        <f>SUM(C75:C79)</f>
+        <v>560</v>
+      </c>
+      <c r="D80">
+        <f t="shared" ref="D80:E80" si="24">SUM(D76:D79)</f>
+        <v>492</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="24"/>
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="81" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="I81" t="s">
+        <v>89</v>
+      </c>
+      <c r="J81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
+        <v>81</v>
+      </c>
+      <c r="E82">
+        <v>1856</v>
+      </c>
+      <c r="K82" t="s">
+        <v>81</v>
+      </c>
+      <c r="L82">
         <v>1706</v>
       </c>
     </row>

</xml_diff>